<commit_message>
commit for 500 run experiment with revo model
</commit_message>
<xml_diff>
--- a/testbook.xlsx
+++ b/testbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\ABM_master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A49A5B-7403-41B7-8305-0517DA91F799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EB7B8F-AB0C-4A64-9BE5-7401525DB966}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="4500" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:G60"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,22 +1104,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B31">
         <v>4000</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E31">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F31">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1127,22 +1127,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B32">
         <v>4000</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E32">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F32">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1150,22 +1150,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B33">
         <v>4000</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D33">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E33">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F33">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1173,22 +1173,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B34">
         <v>4000</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E34">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F34">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1196,22 +1196,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B35">
         <v>4000</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E35">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F35">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -1219,22 +1219,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B36">
         <v>4000</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E36">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F36">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1242,22 +1242,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B37">
         <v>4000</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E37">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F37">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -1265,22 +1265,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B38">
         <v>4000</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E38">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F38">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -1288,22 +1288,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B39">
         <v>4000</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E39">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F39">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -1311,22 +1311,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B40">
         <v>4000</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E40">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F40">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -1334,22 +1334,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B41">
         <v>4000</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E41">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F41">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1357,22 +1357,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B42">
         <v>4000</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D42">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E42">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F42">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -1380,22 +1380,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B43">
         <v>4000</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D43">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E43">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F43">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -1403,22 +1403,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B44">
         <v>4000</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E44">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F44">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -1426,22 +1426,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B45">
         <v>4000</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D45">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E45">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F45">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -1449,22 +1449,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B46">
         <v>4000</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D46">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E46">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F46">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -1472,22 +1472,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B47">
         <v>4000</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E47">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F47">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -1495,22 +1495,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B48">
         <v>4000</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D48">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E48">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F48">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1518,22 +1518,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B49">
         <v>4000</v>
       </c>
       <c r="C49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E49">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F49">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -1541,22 +1541,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="B50">
         <v>4000</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="E50">
-        <v>500</v>
+        <v>-500</v>
       </c>
       <c r="F50">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -1789,6 +1789,926 @@
         <v>150</v>
       </c>
       <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1000</v>
+      </c>
+      <c r="B61">
+        <v>4000</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>50</v>
+      </c>
+      <c r="E61">
+        <v>500</v>
+      </c>
+      <c r="F61">
+        <v>150</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1000</v>
+      </c>
+      <c r="B62">
+        <v>4000</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>50</v>
+      </c>
+      <c r="E62">
+        <v>500</v>
+      </c>
+      <c r="F62">
+        <v>150</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1000</v>
+      </c>
+      <c r="B63">
+        <v>4000</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>50</v>
+      </c>
+      <c r="E63">
+        <v>500</v>
+      </c>
+      <c r="F63">
+        <v>150</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1000</v>
+      </c>
+      <c r="B64">
+        <v>4000</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>50</v>
+      </c>
+      <c r="E64">
+        <v>500</v>
+      </c>
+      <c r="F64">
+        <v>150</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1000</v>
+      </c>
+      <c r="B65">
+        <v>4000</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>50</v>
+      </c>
+      <c r="E65">
+        <v>500</v>
+      </c>
+      <c r="F65">
+        <v>150</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1000</v>
+      </c>
+      <c r="B66">
+        <v>4000</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>50</v>
+      </c>
+      <c r="E66">
+        <v>500</v>
+      </c>
+      <c r="F66">
+        <v>150</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1000</v>
+      </c>
+      <c r="B67">
+        <v>4000</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>50</v>
+      </c>
+      <c r="E67">
+        <v>500</v>
+      </c>
+      <c r="F67">
+        <v>150</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1000</v>
+      </c>
+      <c r="B68">
+        <v>4000</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>50</v>
+      </c>
+      <c r="E68">
+        <v>500</v>
+      </c>
+      <c r="F68">
+        <v>150</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1000</v>
+      </c>
+      <c r="B69">
+        <v>4000</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>50</v>
+      </c>
+      <c r="E69">
+        <v>500</v>
+      </c>
+      <c r="F69">
+        <v>150</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1000</v>
+      </c>
+      <c r="B70">
+        <v>4000</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>50</v>
+      </c>
+      <c r="E70">
+        <v>500</v>
+      </c>
+      <c r="F70">
+        <v>150</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1000</v>
+      </c>
+      <c r="B71">
+        <v>4000</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>50</v>
+      </c>
+      <c r="E71">
+        <v>500</v>
+      </c>
+      <c r="F71">
+        <v>150</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1000</v>
+      </c>
+      <c r="B72">
+        <v>4000</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>50</v>
+      </c>
+      <c r="E72">
+        <v>500</v>
+      </c>
+      <c r="F72">
+        <v>150</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1000</v>
+      </c>
+      <c r="B73">
+        <v>4000</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <v>50</v>
+      </c>
+      <c r="E73">
+        <v>500</v>
+      </c>
+      <c r="F73">
+        <v>150</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1000</v>
+      </c>
+      <c r="B74">
+        <v>4000</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74">
+        <v>50</v>
+      </c>
+      <c r="E74">
+        <v>500</v>
+      </c>
+      <c r="F74">
+        <v>150</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1000</v>
+      </c>
+      <c r="B75">
+        <v>4000</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>50</v>
+      </c>
+      <c r="E75">
+        <v>500</v>
+      </c>
+      <c r="F75">
+        <v>150</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1000</v>
+      </c>
+      <c r="B76">
+        <v>4000</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>50</v>
+      </c>
+      <c r="E76">
+        <v>500</v>
+      </c>
+      <c r="F76">
+        <v>150</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1000</v>
+      </c>
+      <c r="B77">
+        <v>4000</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77">
+        <v>50</v>
+      </c>
+      <c r="E77">
+        <v>500</v>
+      </c>
+      <c r="F77">
+        <v>150</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1000</v>
+      </c>
+      <c r="B78">
+        <v>4000</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78">
+        <v>50</v>
+      </c>
+      <c r="E78">
+        <v>500</v>
+      </c>
+      <c r="F78">
+        <v>150</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1000</v>
+      </c>
+      <c r="B79">
+        <v>4000</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79">
+        <v>50</v>
+      </c>
+      <c r="E79">
+        <v>500</v>
+      </c>
+      <c r="F79">
+        <v>150</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1000</v>
+      </c>
+      <c r="B80">
+        <v>4000</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>50</v>
+      </c>
+      <c r="E80">
+        <v>500</v>
+      </c>
+      <c r="F80">
+        <v>150</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1000</v>
+      </c>
+      <c r="B81">
+        <v>4000</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>50</v>
+      </c>
+      <c r="E81">
+        <v>500</v>
+      </c>
+      <c r="F81">
+        <v>150</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1000</v>
+      </c>
+      <c r="B82">
+        <v>4000</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>50</v>
+      </c>
+      <c r="E82">
+        <v>500</v>
+      </c>
+      <c r="F82">
+        <v>150</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1000</v>
+      </c>
+      <c r="B83">
+        <v>4000</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <v>50</v>
+      </c>
+      <c r="E83">
+        <v>500</v>
+      </c>
+      <c r="F83">
+        <v>150</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>1000</v>
+      </c>
+      <c r="B84">
+        <v>4000</v>
+      </c>
+      <c r="C84">
+        <v>2</v>
+      </c>
+      <c r="D84">
+        <v>50</v>
+      </c>
+      <c r="E84">
+        <v>500</v>
+      </c>
+      <c r="F84">
+        <v>150</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>1000</v>
+      </c>
+      <c r="B85">
+        <v>4000</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+      <c r="D85">
+        <v>50</v>
+      </c>
+      <c r="E85">
+        <v>500</v>
+      </c>
+      <c r="F85">
+        <v>150</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>1000</v>
+      </c>
+      <c r="B86">
+        <v>4000</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>50</v>
+      </c>
+      <c r="E86">
+        <v>500</v>
+      </c>
+      <c r="F86">
+        <v>150</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1000</v>
+      </c>
+      <c r="B87">
+        <v>4000</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87">
+        <v>50</v>
+      </c>
+      <c r="E87">
+        <v>500</v>
+      </c>
+      <c r="F87">
+        <v>150</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1000</v>
+      </c>
+      <c r="B88">
+        <v>4000</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88">
+        <v>50</v>
+      </c>
+      <c r="E88">
+        <v>500</v>
+      </c>
+      <c r="F88">
+        <v>150</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1000</v>
+      </c>
+      <c r="B89">
+        <v>4000</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89">
+        <v>50</v>
+      </c>
+      <c r="E89">
+        <v>500</v>
+      </c>
+      <c r="F89">
+        <v>150</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>1000</v>
+      </c>
+      <c r="B90">
+        <v>4000</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90">
+        <v>50</v>
+      </c>
+      <c r="E90">
+        <v>500</v>
+      </c>
+      <c r="F90">
+        <v>150</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1000</v>
+      </c>
+      <c r="B91">
+        <v>4000</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91">
+        <v>50</v>
+      </c>
+      <c r="E91">
+        <v>500</v>
+      </c>
+      <c r="F91">
+        <v>150</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1000</v>
+      </c>
+      <c r="B92">
+        <v>4000</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <v>50</v>
+      </c>
+      <c r="E92">
+        <v>500</v>
+      </c>
+      <c r="F92">
+        <v>150</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1000</v>
+      </c>
+      <c r="B93">
+        <v>4000</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93">
+        <v>50</v>
+      </c>
+      <c r="E93">
+        <v>500</v>
+      </c>
+      <c r="F93">
+        <v>150</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1000</v>
+      </c>
+      <c r="B94">
+        <v>4000</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94">
+        <v>50</v>
+      </c>
+      <c r="E94">
+        <v>500</v>
+      </c>
+      <c r="F94">
+        <v>150</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>1000</v>
+      </c>
+      <c r="B95">
+        <v>4000</v>
+      </c>
+      <c r="C95">
+        <v>2</v>
+      </c>
+      <c r="D95">
+        <v>50</v>
+      </c>
+      <c r="E95">
+        <v>500</v>
+      </c>
+      <c r="F95">
+        <v>150</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>1000</v>
+      </c>
+      <c r="B96">
+        <v>4000</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="D96">
+        <v>50</v>
+      </c>
+      <c r="E96">
+        <v>500</v>
+      </c>
+      <c r="F96">
+        <v>150</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>1000</v>
+      </c>
+      <c r="B97">
+        <v>4000</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97">
+        <v>50</v>
+      </c>
+      <c r="E97">
+        <v>500</v>
+      </c>
+      <c r="F97">
+        <v>150</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>1000</v>
+      </c>
+      <c r="B98">
+        <v>4000</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98">
+        <v>50</v>
+      </c>
+      <c r="E98">
+        <v>500</v>
+      </c>
+      <c r="F98">
+        <v>150</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>1000</v>
+      </c>
+      <c r="B99">
+        <v>4000</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99">
+        <v>50</v>
+      </c>
+      <c r="E99">
+        <v>500</v>
+      </c>
+      <c r="F99">
+        <v>150</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1000</v>
+      </c>
+      <c r="B100">
+        <v>4000</v>
+      </c>
+      <c r="C100">
+        <v>2</v>
+      </c>
+      <c r="D100">
+        <v>50</v>
+      </c>
+      <c r="E100">
+        <v>500</v>
+      </c>
+      <c r="F100">
+        <v>150</v>
+      </c>
+      <c r="G100">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test with new memory
</commit_message>
<xml_diff>
--- a/testbook.xlsx
+++ b/testbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\ABM_master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E61D318-5461-47C2-B9A3-5B46A102E078}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8B1279-6A44-4865-9882-F32412AC1C9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,15 +404,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J100" sqref="J100"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-1000</v>
       </c>
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1000</v>
       </c>
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-1000</v>
       </c>
@@ -481,7 +481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-1000</v>
       </c>
@@ -504,7 +504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-1000</v>
       </c>
@@ -527,7 +527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-1000</v>
       </c>
@@ -550,7 +550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-1000</v>
       </c>
@@ -573,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-1000</v>
       </c>
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-1000</v>
       </c>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-1000</v>
       </c>
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-1000</v>
       </c>
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-1000</v>
       </c>
@@ -688,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-1000</v>
       </c>
@@ -711,7 +711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-1000</v>
       </c>
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-1000</v>
       </c>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-1000</v>
       </c>
@@ -780,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-1000</v>
       </c>
@@ -803,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-1000</v>
       </c>
@@ -826,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-1000</v>
       </c>
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-1000</v>
       </c>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-1000</v>
       </c>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-1000</v>
       </c>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-1000</v>
       </c>
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-1000</v>
       </c>
@@ -964,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-1000</v>
       </c>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-1000</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-1000</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-1000</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-1000</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-1000</v>
       </c>
@@ -1102,467 +1102,467 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B31">
         <v>4000</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E31">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F31">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B32">
         <v>4000</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E32">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F32">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B33">
         <v>4000</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E33">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F33">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B34">
         <v>4000</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E34">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F34">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B35">
         <v>4000</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E35">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F35">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B36">
         <v>4000</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E36">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F36">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B37">
         <v>4000</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E37">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F37">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B38">
         <v>4000</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D38">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E38">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F38">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B39">
         <v>4000</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E39">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F39">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B40">
         <v>4000</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E40">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F40">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B41">
         <v>4000</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E41">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F41">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B42">
         <v>4000</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E42">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F42">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B43">
         <v>4000</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D43">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E43">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F43">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B44">
         <v>4000</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E44">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F44">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B45">
         <v>4000</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E45">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F45">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B46">
         <v>4000</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D46">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E46">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F46">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B47">
         <v>4000</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D47">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E47">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F47">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B48">
         <v>4000</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E48">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F48">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B49">
         <v>4000</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D49">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E49">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F49">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B50">
         <v>4000</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D50">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E50">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F50">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1000</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1000</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1000</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1000</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1000</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1000</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1000</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1000</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1000</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1000</v>
       </c>
@@ -1789,926 +1789,6 @@
         <v>150</v>
       </c>
       <c r="G60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61">
-        <v>1000</v>
-      </c>
-      <c r="B61">
-        <v>4000</v>
-      </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="D61">
-        <v>50</v>
-      </c>
-      <c r="E61">
-        <v>500</v>
-      </c>
-      <c r="F61">
-        <v>150</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62">
-        <v>1000</v>
-      </c>
-      <c r="B62">
-        <v>4000</v>
-      </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="D62">
-        <v>50</v>
-      </c>
-      <c r="E62">
-        <v>500</v>
-      </c>
-      <c r="F62">
-        <v>150</v>
-      </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63">
-        <v>1000</v>
-      </c>
-      <c r="B63">
-        <v>4000</v>
-      </c>
-      <c r="C63">
-        <v>2</v>
-      </c>
-      <c r="D63">
-        <v>50</v>
-      </c>
-      <c r="E63">
-        <v>500</v>
-      </c>
-      <c r="F63">
-        <v>150</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64">
-        <v>1000</v>
-      </c>
-      <c r="B64">
-        <v>4000</v>
-      </c>
-      <c r="C64">
-        <v>2</v>
-      </c>
-      <c r="D64">
-        <v>50</v>
-      </c>
-      <c r="E64">
-        <v>500</v>
-      </c>
-      <c r="F64">
-        <v>150</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65">
-        <v>1000</v>
-      </c>
-      <c r="B65">
-        <v>4000</v>
-      </c>
-      <c r="C65">
-        <v>2</v>
-      </c>
-      <c r="D65">
-        <v>50</v>
-      </c>
-      <c r="E65">
-        <v>500</v>
-      </c>
-      <c r="F65">
-        <v>150</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66">
-        <v>1000</v>
-      </c>
-      <c r="B66">
-        <v>4000</v>
-      </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-      <c r="D66">
-        <v>50</v>
-      </c>
-      <c r="E66">
-        <v>500</v>
-      </c>
-      <c r="F66">
-        <v>150</v>
-      </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67">
-        <v>1000</v>
-      </c>
-      <c r="B67">
-        <v>4000</v>
-      </c>
-      <c r="C67">
-        <v>2</v>
-      </c>
-      <c r="D67">
-        <v>50</v>
-      </c>
-      <c r="E67">
-        <v>500</v>
-      </c>
-      <c r="F67">
-        <v>150</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68">
-        <v>1000</v>
-      </c>
-      <c r="B68">
-        <v>4000</v>
-      </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
-      <c r="D68">
-        <v>50</v>
-      </c>
-      <c r="E68">
-        <v>500</v>
-      </c>
-      <c r="F68">
-        <v>150</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69">
-        <v>1000</v>
-      </c>
-      <c r="B69">
-        <v>4000</v>
-      </c>
-      <c r="C69">
-        <v>2</v>
-      </c>
-      <c r="D69">
-        <v>50</v>
-      </c>
-      <c r="E69">
-        <v>500</v>
-      </c>
-      <c r="F69">
-        <v>150</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70">
-        <v>1000</v>
-      </c>
-      <c r="B70">
-        <v>4000</v>
-      </c>
-      <c r="C70">
-        <v>2</v>
-      </c>
-      <c r="D70">
-        <v>50</v>
-      </c>
-      <c r="E70">
-        <v>500</v>
-      </c>
-      <c r="F70">
-        <v>150</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71">
-        <v>1000</v>
-      </c>
-      <c r="B71">
-        <v>4000</v>
-      </c>
-      <c r="C71">
-        <v>2</v>
-      </c>
-      <c r="D71">
-        <v>50</v>
-      </c>
-      <c r="E71">
-        <v>500</v>
-      </c>
-      <c r="F71">
-        <v>150</v>
-      </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72">
-        <v>1000</v>
-      </c>
-      <c r="B72">
-        <v>4000</v>
-      </c>
-      <c r="C72">
-        <v>2</v>
-      </c>
-      <c r="D72">
-        <v>50</v>
-      </c>
-      <c r="E72">
-        <v>500</v>
-      </c>
-      <c r="F72">
-        <v>150</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73">
-        <v>1000</v>
-      </c>
-      <c r="B73">
-        <v>4000</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73">
-        <v>50</v>
-      </c>
-      <c r="E73">
-        <v>500</v>
-      </c>
-      <c r="F73">
-        <v>150</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74">
-        <v>1000</v>
-      </c>
-      <c r="B74">
-        <v>4000</v>
-      </c>
-      <c r="C74">
-        <v>2</v>
-      </c>
-      <c r="D74">
-        <v>50</v>
-      </c>
-      <c r="E74">
-        <v>500</v>
-      </c>
-      <c r="F74">
-        <v>150</v>
-      </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75">
-        <v>1000</v>
-      </c>
-      <c r="B75">
-        <v>4000</v>
-      </c>
-      <c r="C75">
-        <v>2</v>
-      </c>
-      <c r="D75">
-        <v>50</v>
-      </c>
-      <c r="E75">
-        <v>500</v>
-      </c>
-      <c r="F75">
-        <v>150</v>
-      </c>
-      <c r="G75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76">
-        <v>1000</v>
-      </c>
-      <c r="B76">
-        <v>4000</v>
-      </c>
-      <c r="C76">
-        <v>2</v>
-      </c>
-      <c r="D76">
-        <v>50</v>
-      </c>
-      <c r="E76">
-        <v>500</v>
-      </c>
-      <c r="F76">
-        <v>150</v>
-      </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77">
-        <v>1000</v>
-      </c>
-      <c r="B77">
-        <v>4000</v>
-      </c>
-      <c r="C77">
-        <v>2</v>
-      </c>
-      <c r="D77">
-        <v>50</v>
-      </c>
-      <c r="E77">
-        <v>500</v>
-      </c>
-      <c r="F77">
-        <v>150</v>
-      </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78">
-        <v>1000</v>
-      </c>
-      <c r="B78">
-        <v>4000</v>
-      </c>
-      <c r="C78">
-        <v>2</v>
-      </c>
-      <c r="D78">
-        <v>50</v>
-      </c>
-      <c r="E78">
-        <v>500</v>
-      </c>
-      <c r="F78">
-        <v>150</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79">
-        <v>1000</v>
-      </c>
-      <c r="B79">
-        <v>4000</v>
-      </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
-      <c r="D79">
-        <v>50</v>
-      </c>
-      <c r="E79">
-        <v>500</v>
-      </c>
-      <c r="F79">
-        <v>150</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80">
-        <v>1000</v>
-      </c>
-      <c r="B80">
-        <v>4000</v>
-      </c>
-      <c r="C80">
-        <v>2</v>
-      </c>
-      <c r="D80">
-        <v>50</v>
-      </c>
-      <c r="E80">
-        <v>500</v>
-      </c>
-      <c r="F80">
-        <v>150</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81">
-        <v>1000</v>
-      </c>
-      <c r="B81">
-        <v>4000</v>
-      </c>
-      <c r="C81">
-        <v>2</v>
-      </c>
-      <c r="D81">
-        <v>50</v>
-      </c>
-      <c r="E81">
-        <v>500</v>
-      </c>
-      <c r="F81">
-        <v>150</v>
-      </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82">
-        <v>1000</v>
-      </c>
-      <c r="B82">
-        <v>4000</v>
-      </c>
-      <c r="C82">
-        <v>2</v>
-      </c>
-      <c r="D82">
-        <v>50</v>
-      </c>
-      <c r="E82">
-        <v>500</v>
-      </c>
-      <c r="F82">
-        <v>150</v>
-      </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83">
-        <v>1000</v>
-      </c>
-      <c r="B83">
-        <v>4000</v>
-      </c>
-      <c r="C83">
-        <v>2</v>
-      </c>
-      <c r="D83">
-        <v>50</v>
-      </c>
-      <c r="E83">
-        <v>500</v>
-      </c>
-      <c r="F83">
-        <v>150</v>
-      </c>
-      <c r="G83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84">
-        <v>1000</v>
-      </c>
-      <c r="B84">
-        <v>4000</v>
-      </c>
-      <c r="C84">
-        <v>2</v>
-      </c>
-      <c r="D84">
-        <v>50</v>
-      </c>
-      <c r="E84">
-        <v>500</v>
-      </c>
-      <c r="F84">
-        <v>150</v>
-      </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85">
-        <v>1000</v>
-      </c>
-      <c r="B85">
-        <v>4000</v>
-      </c>
-      <c r="C85">
-        <v>2</v>
-      </c>
-      <c r="D85">
-        <v>50</v>
-      </c>
-      <c r="E85">
-        <v>500</v>
-      </c>
-      <c r="F85">
-        <v>150</v>
-      </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86">
-        <v>1000</v>
-      </c>
-      <c r="B86">
-        <v>4000</v>
-      </c>
-      <c r="C86">
-        <v>2</v>
-      </c>
-      <c r="D86">
-        <v>50</v>
-      </c>
-      <c r="E86">
-        <v>500</v>
-      </c>
-      <c r="F86">
-        <v>150</v>
-      </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87">
-        <v>1000</v>
-      </c>
-      <c r="B87">
-        <v>4000</v>
-      </c>
-      <c r="C87">
-        <v>2</v>
-      </c>
-      <c r="D87">
-        <v>50</v>
-      </c>
-      <c r="E87">
-        <v>500</v>
-      </c>
-      <c r="F87">
-        <v>150</v>
-      </c>
-      <c r="G87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88">
-        <v>1000</v>
-      </c>
-      <c r="B88">
-        <v>4000</v>
-      </c>
-      <c r="C88">
-        <v>2</v>
-      </c>
-      <c r="D88">
-        <v>50</v>
-      </c>
-      <c r="E88">
-        <v>500</v>
-      </c>
-      <c r="F88">
-        <v>150</v>
-      </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89">
-        <v>1000</v>
-      </c>
-      <c r="B89">
-        <v>4000</v>
-      </c>
-      <c r="C89">
-        <v>2</v>
-      </c>
-      <c r="D89">
-        <v>50</v>
-      </c>
-      <c r="E89">
-        <v>500</v>
-      </c>
-      <c r="F89">
-        <v>150</v>
-      </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90">
-        <v>1000</v>
-      </c>
-      <c r="B90">
-        <v>4000</v>
-      </c>
-      <c r="C90">
-        <v>2</v>
-      </c>
-      <c r="D90">
-        <v>50</v>
-      </c>
-      <c r="E90">
-        <v>500</v>
-      </c>
-      <c r="F90">
-        <v>150</v>
-      </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91">
-        <v>1000</v>
-      </c>
-      <c r="B91">
-        <v>4000</v>
-      </c>
-      <c r="C91">
-        <v>2</v>
-      </c>
-      <c r="D91">
-        <v>50</v>
-      </c>
-      <c r="E91">
-        <v>500</v>
-      </c>
-      <c r="F91">
-        <v>150</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92">
-        <v>1000</v>
-      </c>
-      <c r="B92">
-        <v>4000</v>
-      </c>
-      <c r="C92">
-        <v>2</v>
-      </c>
-      <c r="D92">
-        <v>50</v>
-      </c>
-      <c r="E92">
-        <v>500</v>
-      </c>
-      <c r="F92">
-        <v>150</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93">
-        <v>1000</v>
-      </c>
-      <c r="B93">
-        <v>4000</v>
-      </c>
-      <c r="C93">
-        <v>2</v>
-      </c>
-      <c r="D93">
-        <v>50</v>
-      </c>
-      <c r="E93">
-        <v>500</v>
-      </c>
-      <c r="F93">
-        <v>150</v>
-      </c>
-      <c r="G93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94">
-        <v>1000</v>
-      </c>
-      <c r="B94">
-        <v>4000</v>
-      </c>
-      <c r="C94">
-        <v>2</v>
-      </c>
-      <c r="D94">
-        <v>50</v>
-      </c>
-      <c r="E94">
-        <v>500</v>
-      </c>
-      <c r="F94">
-        <v>150</v>
-      </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95">
-        <v>1000</v>
-      </c>
-      <c r="B95">
-        <v>4000</v>
-      </c>
-      <c r="C95">
-        <v>2</v>
-      </c>
-      <c r="D95">
-        <v>50</v>
-      </c>
-      <c r="E95">
-        <v>500</v>
-      </c>
-      <c r="F95">
-        <v>150</v>
-      </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>1000</v>
-      </c>
-      <c r="B96">
-        <v>4000</v>
-      </c>
-      <c r="C96">
-        <v>2</v>
-      </c>
-      <c r="D96">
-        <v>50</v>
-      </c>
-      <c r="E96">
-        <v>500</v>
-      </c>
-      <c r="F96">
-        <v>150</v>
-      </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97">
-        <v>1000</v>
-      </c>
-      <c r="B97">
-        <v>4000</v>
-      </c>
-      <c r="C97">
-        <v>2</v>
-      </c>
-      <c r="D97">
-        <v>50</v>
-      </c>
-      <c r="E97">
-        <v>500</v>
-      </c>
-      <c r="F97">
-        <v>150</v>
-      </c>
-      <c r="G97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A98">
-        <v>1000</v>
-      </c>
-      <c r="B98">
-        <v>4000</v>
-      </c>
-      <c r="C98">
-        <v>2</v>
-      </c>
-      <c r="D98">
-        <v>50</v>
-      </c>
-      <c r="E98">
-        <v>500</v>
-      </c>
-      <c r="F98">
-        <v>150</v>
-      </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A99">
-        <v>1000</v>
-      </c>
-      <c r="B99">
-        <v>4000</v>
-      </c>
-      <c r="C99">
-        <v>2</v>
-      </c>
-      <c r="D99">
-        <v>50</v>
-      </c>
-      <c r="E99">
-        <v>500</v>
-      </c>
-      <c r="F99">
-        <v>150</v>
-      </c>
-      <c r="G99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100">
-        <v>1000</v>
-      </c>
-      <c r="B100">
-        <v>4000</v>
-      </c>
-      <c r="C100">
-        <v>2</v>
-      </c>
-      <c r="D100">
-        <v>50</v>
-      </c>
-      <c r="E100">
-        <v>500</v>
-      </c>
-      <c r="F100">
-        <v>150</v>
-      </c>
-      <c r="G100">
         <v>0</v>
       </c>
     </row>
@@ -2725,9 +1805,9 @@
       <selection sqref="A1:Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -2780,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2833,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2886,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2939,7 +2019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2992,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -3045,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -3098,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -3151,7 +2231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3204,7 +2284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3257,7 +2337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3310,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3363,7 +2443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -3416,7 +2496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3469,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3522,7 +2602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3575,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -3642,9 +2722,9 @@
       <selection sqref="A1:Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3697,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3750,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3803,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -3856,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -3909,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -3962,7 +3042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4015,7 +3095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4068,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4121,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -4174,7 +3254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -4227,7 +3307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -4280,7 +3360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -4333,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4386,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -4439,7 +3519,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -4492,7 +3572,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -4559,9 +3639,9 @@
       <selection activeCell="H9" sqref="H9:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -4615,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4669,7 +3749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4723,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -4777,7 +3857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -4831,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -4885,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4938,7 +4018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4991,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -5044,7 +4124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -5097,7 +4177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -5150,7 +4230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -5203,7 +4283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -5256,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -5309,7 +4389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -5362,7 +4442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -5415,7 +4495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -5482,9 +4562,9 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -5538,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5591,7 +4671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -5644,7 +4724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -5697,7 +4777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -5750,7 +4830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -5803,7 +4883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -5856,7 +4936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -5909,7 +4989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -5962,7 +5042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -6015,7 +5095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -6069,7 +5149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -6123,7 +5203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -6177,7 +5257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -6231,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -6285,7 +5365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -6338,7 +5418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
new LR cm and memo
</commit_message>
<xml_diff>
--- a/testbook.xlsx
+++ b/testbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\ABM_master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8B1279-6A44-4865-9882-F32412AC1C9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241AF182-C898-4F3C-B678-68075AF4B4F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="A31" sqref="A31:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,22 +759,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B16">
         <v>4000</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E16">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F16">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -782,22 +782,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B17">
         <v>4000</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E17">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F17">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -805,22 +805,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B18">
         <v>4000</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E18">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F18">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -828,22 +828,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B19">
         <v>4000</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E19">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F19">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -851,22 +851,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B20">
         <v>4000</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E20">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F20">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -874,22 +874,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B21">
         <v>4000</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E21">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F21">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -897,22 +897,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B22">
         <v>4000</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E22">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F22">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -920,22 +920,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B23">
         <v>4000</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E23">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F23">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -943,22 +943,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B24">
         <v>4000</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E24">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F24">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -966,22 +966,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B25">
         <v>4000</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E25">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F25">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -989,22 +989,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B26">
         <v>4000</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E26">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F26">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1012,22 +1012,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B27">
         <v>4000</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E27">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F27">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1035,22 +1035,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B28">
         <v>4000</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E28">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F28">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1058,22 +1058,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B29">
         <v>4000</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E29">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F29">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1081,714 +1081,24 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>-1000</v>
+        <v>1000</v>
       </c>
       <c r="B30">
         <v>4000</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>-50</v>
+        <v>50</v>
       </c>
       <c r="E30">
-        <v>-500</v>
+        <v>500</v>
       </c>
       <c r="F30">
-        <v>-150</v>
+        <v>150</v>
       </c>
       <c r="G30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1000</v>
-      </c>
-      <c r="B31">
-        <v>4000</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>50</v>
-      </c>
-      <c r="E31">
-        <v>500</v>
-      </c>
-      <c r="F31">
-        <v>150</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1000</v>
-      </c>
-      <c r="B32">
-        <v>4000</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32">
-        <v>50</v>
-      </c>
-      <c r="E32">
-        <v>500</v>
-      </c>
-      <c r="F32">
-        <v>150</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1000</v>
-      </c>
-      <c r="B33">
-        <v>4000</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
-        <v>50</v>
-      </c>
-      <c r="E33">
-        <v>500</v>
-      </c>
-      <c r="F33">
-        <v>150</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1000</v>
-      </c>
-      <c r="B34">
-        <v>4000</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
-        <v>50</v>
-      </c>
-      <c r="E34">
-        <v>500</v>
-      </c>
-      <c r="F34">
-        <v>150</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1000</v>
-      </c>
-      <c r="B35">
-        <v>4000</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35">
-        <v>50</v>
-      </c>
-      <c r="E35">
-        <v>500</v>
-      </c>
-      <c r="F35">
-        <v>150</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1000</v>
-      </c>
-      <c r="B36">
-        <v>4000</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>50</v>
-      </c>
-      <c r="E36">
-        <v>500</v>
-      </c>
-      <c r="F36">
-        <v>150</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1000</v>
-      </c>
-      <c r="B37">
-        <v>4000</v>
-      </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
-        <v>50</v>
-      </c>
-      <c r="E37">
-        <v>500</v>
-      </c>
-      <c r="F37">
-        <v>150</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1000</v>
-      </c>
-      <c r="B38">
-        <v>4000</v>
-      </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38">
-        <v>50</v>
-      </c>
-      <c r="E38">
-        <v>500</v>
-      </c>
-      <c r="F38">
-        <v>150</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1000</v>
-      </c>
-      <c r="B39">
-        <v>4000</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39">
-        <v>50</v>
-      </c>
-      <c r="E39">
-        <v>500</v>
-      </c>
-      <c r="F39">
-        <v>150</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1000</v>
-      </c>
-      <c r="B40">
-        <v>4000</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40">
-        <v>50</v>
-      </c>
-      <c r="E40">
-        <v>500</v>
-      </c>
-      <c r="F40">
-        <v>150</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1000</v>
-      </c>
-      <c r="B41">
-        <v>4000</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41">
-        <v>50</v>
-      </c>
-      <c r="E41">
-        <v>500</v>
-      </c>
-      <c r="F41">
-        <v>150</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1000</v>
-      </c>
-      <c r="B42">
-        <v>4000</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42">
-        <v>50</v>
-      </c>
-      <c r="E42">
-        <v>500</v>
-      </c>
-      <c r="F42">
-        <v>150</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1000</v>
-      </c>
-      <c r="B43">
-        <v>4000</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43">
-        <v>50</v>
-      </c>
-      <c r="E43">
-        <v>500</v>
-      </c>
-      <c r="F43">
-        <v>150</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1000</v>
-      </c>
-      <c r="B44">
-        <v>4000</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44">
-        <v>50</v>
-      </c>
-      <c r="E44">
-        <v>500</v>
-      </c>
-      <c r="F44">
-        <v>150</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1000</v>
-      </c>
-      <c r="B45">
-        <v>4000</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>50</v>
-      </c>
-      <c r="E45">
-        <v>500</v>
-      </c>
-      <c r="F45">
-        <v>150</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>1000</v>
-      </c>
-      <c r="B46">
-        <v>4000</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46">
-        <v>50</v>
-      </c>
-      <c r="E46">
-        <v>500</v>
-      </c>
-      <c r="F46">
-        <v>150</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>1000</v>
-      </c>
-      <c r="B47">
-        <v>4000</v>
-      </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47">
-        <v>50</v>
-      </c>
-      <c r="E47">
-        <v>500</v>
-      </c>
-      <c r="F47">
-        <v>150</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>1000</v>
-      </c>
-      <c r="B48">
-        <v>4000</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48">
-        <v>50</v>
-      </c>
-      <c r="E48">
-        <v>500</v>
-      </c>
-      <c r="F48">
-        <v>150</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>1000</v>
-      </c>
-      <c r="B49">
-        <v>4000</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49">
-        <v>50</v>
-      </c>
-      <c r="E49">
-        <v>500</v>
-      </c>
-      <c r="F49">
-        <v>150</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>1000</v>
-      </c>
-      <c r="B50">
-        <v>4000</v>
-      </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50">
-        <v>50</v>
-      </c>
-      <c r="E50">
-        <v>500</v>
-      </c>
-      <c r="F50">
-        <v>150</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>1000</v>
-      </c>
-      <c r="B51">
-        <v>4000</v>
-      </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="D51">
-        <v>50</v>
-      </c>
-      <c r="E51">
-        <v>500</v>
-      </c>
-      <c r="F51">
-        <v>150</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>1000</v>
-      </c>
-      <c r="B52">
-        <v>4000</v>
-      </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52">
-        <v>50</v>
-      </c>
-      <c r="E52">
-        <v>500</v>
-      </c>
-      <c r="F52">
-        <v>150</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>1000</v>
-      </c>
-      <c r="B53">
-        <v>4000</v>
-      </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="D53">
-        <v>50</v>
-      </c>
-      <c r="E53">
-        <v>500</v>
-      </c>
-      <c r="F53">
-        <v>150</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>1000</v>
-      </c>
-      <c r="B54">
-        <v>4000</v>
-      </c>
-      <c r="C54">
-        <v>2</v>
-      </c>
-      <c r="D54">
-        <v>50</v>
-      </c>
-      <c r="E54">
-        <v>500</v>
-      </c>
-      <c r="F54">
-        <v>150</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>1000</v>
-      </c>
-      <c r="B55">
-        <v>4000</v>
-      </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55">
-        <v>50</v>
-      </c>
-      <c r="E55">
-        <v>500</v>
-      </c>
-      <c r="F55">
-        <v>150</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>1000</v>
-      </c>
-      <c r="B56">
-        <v>4000</v>
-      </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56">
-        <v>50</v>
-      </c>
-      <c r="E56">
-        <v>500</v>
-      </c>
-      <c r="F56">
-        <v>150</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>1000</v>
-      </c>
-      <c r="B57">
-        <v>4000</v>
-      </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57">
-        <v>50</v>
-      </c>
-      <c r="E57">
-        <v>500</v>
-      </c>
-      <c r="F57">
-        <v>150</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>1000</v>
-      </c>
-      <c r="B58">
-        <v>4000</v>
-      </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58">
-        <v>50</v>
-      </c>
-      <c r="E58">
-        <v>500</v>
-      </c>
-      <c r="F58">
-        <v>150</v>
-      </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>1000</v>
-      </c>
-      <c r="B59">
-        <v>4000</v>
-      </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59">
-        <v>50</v>
-      </c>
-      <c r="E59">
-        <v>500</v>
-      </c>
-      <c r="F59">
-        <v>150</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>1000</v>
-      </c>
-      <c r="B60">
-        <v>4000</v>
-      </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60">
-        <v>50</v>
-      </c>
-      <c r="E60">
-        <v>500</v>
-      </c>
-      <c r="F60">
-        <v>150</v>
-      </c>
-      <c r="G60">
         <v>0</v>
       </c>
     </row>

</xml_diff>